<commit_message>
Mejora de la tabla sintáctica y manejo de errores
</commit_message>
<xml_diff>
--- a/Tabla.xlsx
+++ b/Tabla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\OneDrive\Documentos\University\Archivos\PDF's\Autómatas\Proyecto_compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9940A960-092C-4A72-B417-7AF4F07F5FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA798ED0-1E7F-40EA-87FC-07B02F60F468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{ACD2713D-0E28-406E-BDA3-DABEDB8936F7}"/>
   </bookViews>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FDC48B-7DB9-4621-9590-20BC4BE1981F}">
   <dimension ref="C3:AE24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="58" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -748,7 +748,7 @@
       </c>
     </row>
     <row r="4" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D4" t="s">
@@ -835,7 +835,7 @@
       </c>
     </row>
     <row r="5" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -922,7 +922,7 @@
       </c>
     </row>
     <row r="6" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -1009,7 +1009,7 @@
       </c>
     </row>
     <row r="7" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1096,7 +1096,7 @@
       </c>
     </row>
     <row r="8" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1154,20 +1154,20 @@
       <c r="V8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="W8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>35</v>
+      <c r="W8" t="s">
+        <v>39</v>
+      </c>
+      <c r="X8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>39</v>
       </c>
       <c r="AB8" t="s">
         <v>33</v>
@@ -1183,7 +1183,7 @@
       </c>
     </row>
     <row r="9" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -1270,7 +1270,7 @@
       </c>
     </row>
     <row r="10" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -1357,7 +1357,7 @@
       </c>
     </row>
     <row r="11" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -1444,7 +1444,7 @@
       </c>
     </row>
     <row r="12" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -1531,7 +1531,7 @@
       </c>
     </row>
     <row r="13" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -1618,7 +1618,7 @@
       </c>
     </row>
     <row r="14" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -1705,7 +1705,7 @@
       </c>
     </row>
     <row r="15" spans="3:31" x14ac:dyDescent="0.45">
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="4" t="s">

</xml_diff>

<commit_message>
Implementación de Tabla de Símbolos
</commit_message>
<xml_diff>
--- a/Tabla.xlsx
+++ b/Tabla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\OneDrive\Documentos\University\Archivos\PDF's\Autómatas\Proyecto_compilador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E845C58-93AA-4133-A071-0D5A7F015B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5ABA87-C58F-404E-ACBD-0C0D3E2169AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{ACD2713D-0E28-406E-BDA3-DABEDB8936F7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="167">
   <si>
     <t>id</t>
   </si>
@@ -465,9 +465,6 @@
     <t xml:space="preserve"> % FT'</t>
   </si>
   <si>
-    <t>, F</t>
-  </si>
-  <si>
     <t>$L'R'E'T')L'R'E'F,</t>
   </si>
   <si>
@@ -493,6 +490,51 @@
   </si>
   <si>
     <t>return L;</t>
+  </si>
+  <si>
+    <t>EN TODAS LA DE SENTENCIA A SIGARG PONLE CADENA VACIA</t>
+  </si>
+  <si>
+    <t>endprogram SENT DEC MOD ) LISTA_ARG ( idProgram program</t>
+  </si>
+  <si>
+    <t>program Nuevo (int c, )</t>
+  </si>
+  <si>
+    <t>endprogram SENT DEC MOD ) LISTA_ARG ( idProgram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endprogram SENT DEC MOD ) LISTA_ARG ( </t>
+  </si>
+  <si>
+    <t>concuerda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endprogram SENT DEC MOD ) LISTA_ARG </t>
+  </si>
+  <si>
+    <t>endprogram SENT DEC MOD ) SIGARG id int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t xml:space="preserve">endprogram SENT DEC MOD ) SIGARG id </t>
+  </si>
+  <si>
+    <t>endprogram SENT DEC MOD ) SIGARG</t>
+  </si>
+  <si>
+    <t>endprogram SENT DEC MOD ) LISTA_ARG ,</t>
+  </si>
+  <si>
+    <t>endprogram SENT DEC MOD ) LISTA_ARG</t>
+  </si>
+  <si>
+    <t>en saltar te quedas  en ese estado hasta que encuentres el valido</t>
+  </si>
+  <si>
+    <t>en func funciona en pro no</t>
   </si>
 </sst>
 </file>
@@ -555,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -587,11 +629,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FDC48B-7DB9-4621-9590-20BC4BE1981F}">
-  <dimension ref="C3:AZ43"/>
+  <dimension ref="C3:BA43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="86" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -942,20 +990,20 @@
     <col min="24" max="24" width="26.73046875" customWidth="1"/>
     <col min="25" max="26" width="10.3984375" customWidth="1"/>
     <col min="27" max="27" width="10.6640625" customWidth="1"/>
-    <col min="28" max="28" width="10.796875" customWidth="1"/>
-    <col min="34" max="36" width="10.86328125" customWidth="1"/>
-    <col min="37" max="37" width="10.796875" customWidth="1"/>
-    <col min="38" max="38" width="11.59765625" customWidth="1"/>
-    <col min="39" max="39" width="10.59765625" customWidth="1"/>
-    <col min="40" max="40" width="11.265625" customWidth="1"/>
-    <col min="41" max="41" width="11" customWidth="1"/>
-    <col min="42" max="43" width="11.19921875" customWidth="1"/>
-    <col min="44" max="44" width="11.53125" customWidth="1"/>
-    <col min="45" max="48" width="10.6640625" customWidth="1"/>
-    <col min="49" max="49" width="11.1328125" customWidth="1"/>
+    <col min="28" max="29" width="10.796875" customWidth="1"/>
+    <col min="35" max="37" width="10.86328125" customWidth="1"/>
+    <col min="38" max="38" width="10.796875" customWidth="1"/>
+    <col min="39" max="39" width="11.59765625" customWidth="1"/>
+    <col min="40" max="40" width="10.59765625" customWidth="1"/>
+    <col min="41" max="41" width="11.265625" customWidth="1"/>
+    <col min="42" max="42" width="11" customWidth="1"/>
+    <col min="43" max="44" width="11.19921875" customWidth="1"/>
+    <col min="45" max="45" width="11.53125" customWidth="1"/>
+    <col min="46" max="49" width="10.6640625" customWidth="1"/>
+    <col min="50" max="50" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:52" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="3:53" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C3" s="13"/>
       <c r="D3" s="15" t="s">
         <v>115</v>
@@ -1032,80 +1080,83 @@
       <c r="AB3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="AC3" s="15" t="s">
+      <c r="AC3" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="AD3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AE3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="AE3" s="15" t="s">
+      <c r="AF3" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="AF3" s="15" t="s">
+      <c r="AG3" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="AG3" s="15" t="s">
+      <c r="AH3" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="AH3" s="18" t="s">
+      <c r="AI3" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="AI3" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ3" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="AK3" s="15" t="s">
+      <c r="AJ3" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK3" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="AL3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="AL3" s="15" t="s">
+      <c r="AM3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="AM3" s="15" t="s">
+      <c r="AN3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="AN3" s="15" t="s">
+      <c r="AO3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="AO3" s="15" t="s">
+      <c r="AP3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="AP3" s="15" t="s">
+      <c r="AQ3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="AQ3" s="15" t="s">
+      <c r="AR3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="AR3" s="15" t="s">
+      <c r="AS3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="AS3" s="15" t="s">
+      <c r="AT3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="AT3" s="15" t="s">
+      <c r="AU3" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="AU3" s="15" t="s">
+      <c r="AV3" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="AV3" s="15" t="s">
+      <c r="AW3" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="AW3" s="15" t="s">
+      <c r="AX3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="AX3" s="15" t="s">
+      <c r="AY3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="AY3" s="15" t="s">
+      <c r="AZ3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="AZ3" s="15" t="s">
+      <c r="BA3" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="3:52" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="3:53" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C4" s="13" t="s">
         <v>114</v>
       </c>
@@ -1184,9 +1235,7 @@
       <c r="AB4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC4" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC4" s="19"/>
       <c r="AD4" s="2" t="s">
         <v>35</v>
       </c>
@@ -1199,14 +1248,16 @@
       <c r="AG4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AH4" s="16" t="s">
+      <c r="AH4" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AI4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="2" t="s">
+      <c r="AJ4" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK4" s="16" t="s">
         <v>35</v>
       </c>
       <c r="AL4" s="2" t="s">
@@ -1252,10 +1303,13 @@
         <v>35</v>
       </c>
       <c r="AZ4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="3:52" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="3:53" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C5" s="13" t="s">
         <v>97</v>
       </c>
@@ -1334,9 +1388,7 @@
       <c r="AB5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC5" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC5" s="19"/>
       <c r="AD5" s="2" t="s">
         <v>35</v>
       </c>
@@ -1349,18 +1401,20 @@
       <c r="AG5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AH5" s="16" t="s">
+      <c r="AH5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AI5" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AJ5" s="16"/>
-      <c r="AK5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>35</v>
+      <c r="AJ5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="AM5" s="2" t="s">
         <v>35</v>
@@ -1402,10 +1456,13 @@
         <v>35</v>
       </c>
       <c r="AZ5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA5" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="3:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:53" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C6" s="14" t="s">
         <v>101</v>
       </c>
@@ -1418,7 +1475,7 @@
       <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="18" t="s">
         <v>35</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1427,7 +1484,7 @@
       <c r="I6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="18" t="s">
         <v>35</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -1484,9 +1541,7 @@
       <c r="AB6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC6" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC6" s="19"/>
       <c r="AD6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1499,21 +1554,23 @@
       <c r="AG6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AH6" s="16" t="s">
+      <c r="AH6" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AI6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="2" t="s">
+      <c r="AJ6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK6" s="16" t="s">
         <v>35</v>
       </c>
       <c r="AL6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AM6" s="2" t="s">
-        <v>35</v>
+      <c r="AM6" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="AN6" s="2" t="s">
         <v>35</v>
@@ -1552,10 +1609,13 @@
         <v>35</v>
       </c>
       <c r="AZ6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="3:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="3:53" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C7" s="14" t="s">
         <v>102</v>
       </c>
@@ -1634,9 +1694,7 @@
       <c r="AB7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC7" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC7" s="19"/>
       <c r="AD7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1649,21 +1707,23 @@
       <c r="AG7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AH7" s="16" t="s">
+      <c r="AH7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AI7" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AJ7" s="16"/>
-      <c r="AK7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM7" s="2" t="s">
-        <v>35</v>
+      <c r="AJ7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AK7" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM7" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="AN7" s="2" t="s">
         <v>35</v>
@@ -1702,10 +1762,13 @@
         <v>35</v>
       </c>
       <c r="AZ7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA7" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="3:52" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:53" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="C8" s="14" t="s">
         <v>110</v>
       </c>
@@ -1784,9 +1847,7 @@
       <c r="AB8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC8" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC8" s="19"/>
       <c r="AD8" s="2" t="s">
         <v>35</v>
       </c>
@@ -1799,14 +1860,16 @@
       <c r="AG8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AH8" s="16" t="s">
+      <c r="AH8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AI8" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="AJ8" s="16"/>
-      <c r="AK8" s="2" t="s">
+      <c r="AJ8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK8" s="16" t="s">
         <v>35</v>
       </c>
       <c r="AL8" s="2" t="s">
@@ -1852,10 +1915,13 @@
         <v>35</v>
       </c>
       <c r="AZ8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C9" s="13" t="s">
         <v>66</v>
       </c>
@@ -1934,23 +2000,21 @@
       <c r="AB9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC9" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC9" s="19"/>
       <c r="AD9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AE9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AF9" s="4" t="s">
+      <c r="AF9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AG9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AH9" s="1" t="s">
-        <v>31</v>
+      <c r="AH9" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="AI9" s="1" t="s">
         <v>31</v>
@@ -1958,8 +2022,8 @@
       <c r="AJ9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AK9" s="2" t="s">
-        <v>35</v>
+      <c r="AK9" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="AL9" s="2" t="s">
         <v>35</v>
@@ -2004,10 +2068,13 @@
         <v>35</v>
       </c>
       <c r="AZ9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA9" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C10" s="13" t="s">
         <v>85</v>
       </c>
@@ -2086,16 +2153,14 @@
       <c r="AB10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AC10" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC10" s="19"/>
       <c r="AD10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AF10" s="4" t="s">
+      <c r="AF10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AG10" s="4" t="s">
@@ -2107,8 +2172,10 @@
       <c r="AI10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ10" s="4"/>
-      <c r="AK10" s="2" t="s">
+      <c r="AJ10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AL10" s="2" t="s">
@@ -2154,10 +2221,13 @@
         <v>35</v>
       </c>
       <c r="AZ10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA10" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C11" s="13" t="s">
         <v>51</v>
       </c>
@@ -2236,33 +2306,31 @@
       <c r="AB11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AC11" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC11" s="19"/>
       <c r="AD11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AE11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AF11" s="4" t="s">
+      <c r="AF11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AG11" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AH11" s="4" t="s">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="AI11" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AJ11" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AK11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AK11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="AL11" s="2" t="s">
         <v>35</v>
       </c>
@@ -2306,10 +2374,13 @@
         <v>35</v>
       </c>
       <c r="AZ11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C12" s="13" t="s">
         <v>61</v>
       </c>
@@ -2388,16 +2459,13 @@
       <c r="AB12" t="s">
         <v>35</v>
       </c>
-      <c r="AC12" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="AD12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AE12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AF12" s="4" t="s">
+      <c r="AF12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AG12" s="4" t="s">
@@ -2409,14 +2477,16 @@
       <c r="AI12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" t="s">
+      <c r="AJ12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AL12" t="s">
         <v>35</v>
       </c>
-      <c r="AM12" s="2" t="s">
+      <c r="AM12" t="s">
         <v>35</v>
       </c>
       <c r="AN12" s="2" t="s">
@@ -2425,13 +2495,13 @@
       <c r="AO12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AP12" t="s">
+      <c r="AP12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AQ12" t="s">
         <v>35</v>
       </c>
-      <c r="AR12" s="2" t="s">
+      <c r="AR12" t="s">
         <v>35</v>
       </c>
       <c r="AS12" s="2" t="s">
@@ -2440,13 +2510,13 @@
       <c r="AT12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AU12" t="s">
+      <c r="AU12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AV12" t="s">
         <v>35</v>
       </c>
-      <c r="AW12" s="2" t="s">
+      <c r="AW12" t="s">
         <v>35</v>
       </c>
       <c r="AX12" s="2" t="s">
@@ -2456,10 +2526,13 @@
         <v>35</v>
       </c>
       <c r="AZ12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA12" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C13" s="13" t="s">
         <v>45</v>
       </c>
@@ -2538,16 +2611,14 @@
       <c r="AB13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AC13" s="2" t="s">
-        <v>35</v>
-      </c>
+      <c r="AC13" s="19"/>
       <c r="AD13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AE13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AF13" s="4" t="s">
+      <c r="AF13" s="2" t="s">
         <v>35</v>
       </c>
       <c r="AG13" s="4" t="s">
@@ -2559,8 +2630,10 @@
       <c r="AI13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="2" t="s">
+      <c r="AJ13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="AL13" s="2" t="s">
@@ -2606,10 +2679,13 @@
         <v>35</v>
       </c>
       <c r="AZ13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C14" s="13" t="s">
         <v>10</v>
       </c>
@@ -2688,16 +2764,13 @@
       <c r="AB14" t="s">
         <v>19</v>
       </c>
-      <c r="AC14" t="s">
-        <v>19</v>
-      </c>
       <c r="AD14" t="s">
         <v>19</v>
       </c>
       <c r="AE14" t="s">
         <v>19</v>
       </c>
-      <c r="AF14" s="6" t="s">
+      <c r="AF14" t="s">
         <v>19</v>
       </c>
       <c r="AG14" s="6" t="s">
@@ -2712,11 +2785,11 @@
       <c r="AJ14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="AK14" t="s">
+      <c r="AK14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="AL14" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="AM14" t="s">
         <v>35</v>
@@ -2755,13 +2828,16 @@
         <v>35</v>
       </c>
       <c r="AY14" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ14" t="s">
         <v>30</v>
       </c>
-      <c r="AZ14" t="s">
+      <c r="BA14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C15" s="13" t="s">
         <v>11</v>
       </c>
@@ -2840,16 +2916,13 @@
       <c r="AB15" t="s">
         <v>35</v>
       </c>
-      <c r="AC15" t="s">
-        <v>35</v>
-      </c>
       <c r="AD15" t="s">
         <v>35</v>
       </c>
       <c r="AE15" t="s">
         <v>35</v>
       </c>
-      <c r="AF15" s="6" t="s">
+      <c r="AF15" t="s">
         <v>35</v>
       </c>
       <c r="AG15" s="6" t="s">
@@ -2861,12 +2934,14 @@
       <c r="AI15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ15" s="6"/>
-      <c r="AK15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL15" s="1" t="s">
-        <v>31</v>
+      <c r="AJ15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK15" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL15" t="s">
+        <v>35</v>
       </c>
       <c r="AM15" s="1" t="s">
         <v>31</v>
@@ -2883,8 +2958,8 @@
       <c r="AQ15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AR15" t="s">
-        <v>35</v>
+      <c r="AR15" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="AS15" t="s">
         <v>35</v>
@@ -2899,19 +2974,22 @@
         <v>35</v>
       </c>
       <c r="AW15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX15" t="s">
         <v>29</v>
       </c>
-      <c r="AX15" s="1" t="s">
+      <c r="AY15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AY15" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AZ15" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="BA15" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="16" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C16" s="13" t="s">
         <v>12</v>
       </c>
@@ -2990,16 +3068,13 @@
       <c r="AB16" t="s">
         <v>20</v>
       </c>
-      <c r="AC16" t="s">
-        <v>20</v>
-      </c>
       <c r="AD16" t="s">
         <v>20</v>
       </c>
       <c r="AE16" t="s">
         <v>20</v>
       </c>
-      <c r="AF16" s="6" t="s">
+      <c r="AF16" t="s">
         <v>20</v>
       </c>
       <c r="AG16" s="6" t="s">
@@ -3014,11 +3089,11 @@
       <c r="AJ16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AK16" t="s">
+      <c r="AK16" s="6" t="s">
         <v>20</v>
       </c>
       <c r="AL16" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="AM16" t="s">
         <v>35</v>
@@ -3060,10 +3135,13 @@
         <v>35</v>
       </c>
       <c r="AZ16" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="17" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C17" s="13" t="s">
         <v>13</v>
       </c>
@@ -3142,16 +3220,13 @@
       <c r="AB17" t="s">
         <v>35</v>
       </c>
-      <c r="AC17" t="s">
-        <v>35</v>
-      </c>
       <c r="AD17" t="s">
         <v>35</v>
       </c>
       <c r="AE17" t="s">
         <v>35</v>
       </c>
-      <c r="AF17" s="6" t="s">
+      <c r="AF17" t="s">
         <v>35</v>
       </c>
       <c r="AG17" s="6" t="s">
@@ -3163,12 +3238,14 @@
       <c r="AI17" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ17" s="6"/>
-      <c r="AK17" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL17" s="1" t="s">
-        <v>31</v>
+      <c r="AJ17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>35</v>
       </c>
       <c r="AM17" s="1" t="s">
         <v>31</v>
@@ -3185,24 +3262,24 @@
       <c r="AQ17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AR17" t="s">
+      <c r="AR17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AS17" t="s">
         <v>24</v>
       </c>
-      <c r="AS17" t="s">
+      <c r="AT17" t="s">
         <v>25</v>
       </c>
-      <c r="AT17" s="1" t="s">
+      <c r="AU17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AU17" s="1" t="s">
+      <c r="AV17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AV17" s="1" t="s">
+      <c r="AW17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AW17" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AX17" s="1" t="s">
         <v>31</v>
       </c>
@@ -3212,8 +3289,11 @@
       <c r="AZ17" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="BA17" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="18" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C18" s="13" t="s">
         <v>14</v>
       </c>
@@ -3292,16 +3372,13 @@
       <c r="AB18" t="s">
         <v>21</v>
       </c>
-      <c r="AC18" t="s">
-        <v>21</v>
-      </c>
       <c r="AD18" t="s">
         <v>21</v>
       </c>
       <c r="AE18" t="s">
         <v>21</v>
       </c>
-      <c r="AF18" s="6" t="s">
+      <c r="AF18" t="s">
         <v>21</v>
       </c>
       <c r="AG18" s="6" t="s">
@@ -3316,11 +3393,11 @@
       <c r="AJ18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="AK18" t="s">
+      <c r="AK18" s="6" t="s">
         <v>21</v>
       </c>
       <c r="AL18" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="AM18" t="s">
         <v>35</v>
@@ -3362,10 +3439,13 @@
         <v>35</v>
       </c>
       <c r="AZ18" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C19" s="13" t="s">
         <v>15</v>
       </c>
@@ -3444,16 +3524,13 @@
       <c r="AB19" t="s">
         <v>35</v>
       </c>
-      <c r="AC19" t="s">
-        <v>35</v>
-      </c>
       <c r="AD19" t="s">
         <v>35</v>
       </c>
       <c r="AE19" t="s">
         <v>35</v>
       </c>
-      <c r="AF19" s="6" t="s">
+      <c r="AF19" t="s">
         <v>35</v>
       </c>
       <c r="AG19" s="6" t="s">
@@ -3465,22 +3542,24 @@
       <c r="AI19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM19" t="s">
+      <c r="AJ19" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>35</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN19" t="s">
         <v>138</v>
       </c>
-      <c r="AN19" t="s">
+      <c r="AO19" t="s">
         <v>139</v>
       </c>
-      <c r="AO19" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AP19" s="1" t="s">
         <v>31</v>
       </c>
@@ -3514,8 +3593,11 @@
       <c r="AZ19" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="BA19" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="20" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C20" s="13" t="s">
         <v>16</v>
       </c>
@@ -3594,16 +3676,13 @@
       <c r="AB20" t="s">
         <v>22</v>
       </c>
-      <c r="AC20" t="s">
-        <v>22</v>
-      </c>
       <c r="AD20" t="s">
         <v>22</v>
       </c>
       <c r="AE20" t="s">
         <v>22</v>
       </c>
-      <c r="AF20" s="6" t="s">
+      <c r="AF20" t="s">
         <v>22</v>
       </c>
       <c r="AG20" s="6" t="s">
@@ -3618,11 +3697,11 @@
       <c r="AJ20" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="AK20" t="s">
+      <c r="AK20" s="6" t="s">
         <v>22</v>
       </c>
       <c r="AL20" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="AM20" t="s">
         <v>35</v>
@@ -3664,10 +3743,13 @@
         <v>35</v>
       </c>
       <c r="AZ20" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="21" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C21" s="13" t="s">
         <v>17</v>
       </c>
@@ -3717,7 +3799,7 @@
         <v>35</v>
       </c>
       <c r="S21" s="9" t="s">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="T21" s="2" t="s">
         <v>35</v>
@@ -3746,16 +3828,13 @@
       <c r="AB21" t="s">
         <v>35</v>
       </c>
-      <c r="AC21" t="s">
-        <v>35</v>
-      </c>
       <c r="AD21" t="s">
         <v>35</v>
       </c>
       <c r="AE21" t="s">
         <v>35</v>
       </c>
-      <c r="AF21" s="6" t="s">
+      <c r="AF21" t="s">
         <v>35</v>
       </c>
       <c r="AG21" s="6" t="s">
@@ -3767,12 +3846,14 @@
       <c r="AI21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AJ21" s="6"/>
-      <c r="AK21" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL21" s="1" t="s">
-        <v>31</v>
+      <c r="AJ21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>35</v>
       </c>
       <c r="AM21" s="1" t="s">
         <v>31</v>
@@ -3780,18 +3861,18 @@
       <c r="AN21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AO21" t="s">
+      <c r="AO21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP21" t="s">
         <v>140</v>
       </c>
-      <c r="AP21" t="s">
+      <c r="AQ21" t="s">
         <v>141</v>
       </c>
-      <c r="AQ21" t="s">
+      <c r="AR21" t="s">
         <v>142</v>
       </c>
-      <c r="AR21" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="AS21" s="1" t="s">
         <v>31</v>
       </c>
@@ -3816,8 +3897,11 @@
       <c r="AZ21" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="BA21" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="22" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="22" spans="3:53" x14ac:dyDescent="0.45">
       <c r="C22" s="13" t="s">
         <v>18</v>
       </c>
@@ -3896,36 +3980,33 @@
       <c r="AB22" t="s">
         <v>0</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="AD22" t="s">
         <v>1</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>37</v>
       </c>
-      <c r="AE22" t="s">
+      <c r="AF22" t="s">
         <v>38</v>
       </c>
-      <c r="AF22" s="6" t="s">
+      <c r="AG22" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AG22" s="6" t="s">
+      <c r="AH22" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AH22" s="6" t="s">
-        <v>147</v>
-      </c>
       <c r="AI22" s="6" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="AJ22" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="AK22" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK22" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="AL22" t="s">
         <v>23</v>
       </c>
-      <c r="AL22" t="s">
-        <v>35</v>
-      </c>
       <c r="AM22" t="s">
         <v>35</v>
       </c>
@@ -3966,10 +4047,13 @@
         <v>35</v>
       </c>
       <c r="AZ22" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="23" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D23" s="2"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
@@ -3984,10 +4068,13 @@
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
     </row>
-    <row r="24" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="25" spans="3:53" x14ac:dyDescent="0.45">
+      <c r="C25" s="13" t="s">
+        <v>152</v>
+      </c>
       <c r="D25" s="2"/>
       <c r="T25" s="2"/>
       <c r="X25" t="s">
@@ -3999,31 +4086,49 @@
       <c r="AB25" t="b">
         <v>1</v>
       </c>
-      <c r="AC25" t="b">
+      <c r="AD25" t="b">
         <v>0</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D26" s="2"/>
+      <c r="I26" t="s">
+        <v>154</v>
+      </c>
       <c r="W26" t="s">
         <v>51</v>
       </c>
       <c r="AB26" t="s">
         <v>48</v>
       </c>
-      <c r="AL26" s="17" t="s">
+      <c r="AM26" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="AM26" s="17"/>
-      <c r="AN26" t="s">
+      <c r="AN26" s="20"/>
+      <c r="AO26" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D27" s="2"/>
+      <c r="F27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" t="s">
+        <v>115</v>
+      </c>
+      <c r="J27" t="s">
+        <v>157</v>
+      </c>
+      <c r="S27" t="s">
+        <v>166</v>
+      </c>
       <c r="W27" t="s">
         <v>51</v>
       </c>
@@ -4033,33 +4138,69 @@
       <c r="AB27" t="s">
         <v>49</v>
       </c>
-      <c r="AL27" s="17" t="s">
+      <c r="AM27" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="AM27" s="17"/>
+      <c r="AN27" s="20"/>
     </row>
-    <row r="28" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D28" s="2"/>
+      <c r="F28" t="s">
+        <v>114</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="I28" t="s">
+        <v>118</v>
+      </c>
+      <c r="J28" t="s">
+        <v>157</v>
+      </c>
       <c r="W28" t="s">
         <v>74</v>
       </c>
-      <c r="AL28" s="17" t="s">
+      <c r="AM28" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="AM28" s="17"/>
+      <c r="AN28" s="20"/>
     </row>
-    <row r="29" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D29" s="2"/>
+      <c r="F29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I29" t="s">
+        <v>2</v>
+      </c>
+      <c r="J29" t="s">
+        <v>157</v>
+      </c>
       <c r="W29" t="s">
         <v>75</v>
       </c>
-      <c r="AL29" s="17" t="s">
+      <c r="AM29" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="AM29" s="17"/>
+      <c r="AN29" s="20"/>
     </row>
-    <row r="30" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:53" x14ac:dyDescent="0.45">
       <c r="D30" s="2"/>
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I30" t="s">
+        <v>160</v>
+      </c>
+      <c r="J30" t="s">
+        <v>157</v>
+      </c>
       <c r="W30" t="s">
         <v>75</v>
       </c>
@@ -4069,12 +4210,19 @@
       <c r="AB30" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AL30" s="17" t="s">
+      <c r="AC30" s="3"/>
+      <c r="AM30" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="AM30" s="17"/>
+      <c r="AN30" s="20"/>
     </row>
-    <row r="31" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:53" x14ac:dyDescent="0.45">
+      <c r="F31" t="s">
+        <v>101</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>159</v>
+      </c>
       <c r="W31" t="s">
         <v>76</v>
       </c>
@@ -4084,124 +4232,167 @@
       <c r="AB31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AD31" t="s">
+      <c r="AC31" s="3"/>
+      <c r="AE31" t="s">
         <v>96</v>
       </c>
-      <c r="AL31" s="17" t="s">
+      <c r="AM31" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="AM31" s="17"/>
+      <c r="AN31" s="20"/>
     </row>
-    <row r="32" spans="3:52" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:53" x14ac:dyDescent="0.45">
+      <c r="F32" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="I32" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" t="s">
+        <v>157</v>
+      </c>
       <c r="W32" t="s">
         <v>76</v>
       </c>
-      <c r="AL32" s="17" t="s">
+      <c r="AM32" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="AM32" s="17"/>
+      <c r="AN32" s="20"/>
     </row>
-    <row r="33" spans="23:39" x14ac:dyDescent="0.45">
+    <row r="33" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="F33" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>162</v>
+      </c>
       <c r="W33" t="s">
         <v>80</v>
       </c>
-      <c r="AL33" s="17" t="s">
+      <c r="AM33" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="AM33" s="17"/>
+      <c r="AN33" s="20"/>
     </row>
-    <row r="34" spans="23:39" x14ac:dyDescent="0.45">
+    <row r="34" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="F34" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I34" t="s">
+        <v>90</v>
+      </c>
+      <c r="J34" t="s">
+        <v>157</v>
+      </c>
       <c r="W34" t="s">
         <v>81</v>
       </c>
-      <c r="AL34" s="17" t="s">
+      <c r="AM34" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="AM34" s="17"/>
+      <c r="AN34" s="20"/>
     </row>
-    <row r="35" spans="23:39" x14ac:dyDescent="0.45">
+    <row r="35" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="F35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I35" t="s">
+        <v>3</v>
+      </c>
       <c r="W35" t="s">
         <v>82</v>
       </c>
-      <c r="AL35" s="17" t="s">
+      <c r="AM35" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="AM35" s="17"/>
+      <c r="AN35" s="20"/>
     </row>
-    <row r="36" spans="23:39" x14ac:dyDescent="0.45">
+    <row r="36" spans="6:40" x14ac:dyDescent="0.45">
       <c r="W36" t="s">
         <v>83</v>
       </c>
-      <c r="AL36" s="17" t="s">
+      <c r="AM36" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="AM36" s="17"/>
+      <c r="AN36" s="20"/>
     </row>
-    <row r="37" spans="23:39" x14ac:dyDescent="0.45">
+    <row r="37" spans="6:40" x14ac:dyDescent="0.45">
       <c r="W37" t="s">
         <v>84</v>
       </c>
-      <c r="AL37" s="17" t="s">
+      <c r="AM37" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="AM37" s="17"/>
+      <c r="AN37" s="20"/>
     </row>
-    <row r="38" spans="23:39" x14ac:dyDescent="0.45">
-      <c r="AL38" s="17" t="s">
+    <row r="38" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="AM38" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="AM38" s="17"/>
+      <c r="AN38" s="20"/>
     </row>
-    <row r="39" spans="23:39" x14ac:dyDescent="0.45">
-      <c r="AL39" s="17" t="s">
+    <row r="39" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="AM39" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="AM39" s="17"/>
+      <c r="AN39" s="20"/>
     </row>
-    <row r="40" spans="23:39" x14ac:dyDescent="0.45">
-      <c r="AL40" s="17" t="s">
+    <row r="40" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="G40" t="s">
+        <v>165</v>
+      </c>
+      <c r="AM40" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="AN40" s="20"/>
+    </row>
+    <row r="41" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="AM41" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="AM40" s="17"/>
+      <c r="AN41" s="20"/>
     </row>
-    <row r="41" spans="23:39" x14ac:dyDescent="0.45">
-      <c r="AL41" s="17" t="s">
+    <row r="42" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="AM42" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="AM41" s="17"/>
+      <c r="AN42" s="20"/>
     </row>
-    <row r="42" spans="23:39" x14ac:dyDescent="0.45">
-      <c r="AL42" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="AM42" s="17"/>
-    </row>
-    <row r="43" spans="23:39" x14ac:dyDescent="0.45">
-      <c r="AL43" s="17" t="s">
+    <row r="43" spans="6:40" x14ac:dyDescent="0.45">
+      <c r="AM43" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="AM43" s="17"/>
+      <c r="AN43" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AL40:AM40"/>
-    <mergeCell ref="AL41:AM41"/>
-    <mergeCell ref="AL42:AM42"/>
-    <mergeCell ref="AL43:AM43"/>
-    <mergeCell ref="AL26:AM26"/>
-    <mergeCell ref="AL27:AM27"/>
-    <mergeCell ref="AL28:AM28"/>
-    <mergeCell ref="AL29:AM29"/>
-    <mergeCell ref="AL30:AM30"/>
-    <mergeCell ref="AL31:AM31"/>
-    <mergeCell ref="AL32:AM32"/>
-    <mergeCell ref="AL33:AM33"/>
-    <mergeCell ref="AL34:AM34"/>
-    <mergeCell ref="AL35:AM35"/>
-    <mergeCell ref="AL36:AM36"/>
-    <mergeCell ref="AL37:AM37"/>
-    <mergeCell ref="AL38:AM38"/>
-    <mergeCell ref="AL39:AM39"/>
+    <mergeCell ref="AM39:AN39"/>
+    <mergeCell ref="AM40:AN40"/>
+    <mergeCell ref="AM41:AN41"/>
+    <mergeCell ref="AM42:AN42"/>
+    <mergeCell ref="AM43:AN43"/>
+    <mergeCell ref="AM26:AN26"/>
+    <mergeCell ref="AM27:AN27"/>
+    <mergeCell ref="AM28:AN28"/>
+    <mergeCell ref="AM29:AN29"/>
+    <mergeCell ref="AM30:AN30"/>
+    <mergeCell ref="AM36:AN36"/>
+    <mergeCell ref="AM37:AN37"/>
+    <mergeCell ref="AM38:AN38"/>
+    <mergeCell ref="AM31:AN31"/>
+    <mergeCell ref="AM32:AN32"/>
+    <mergeCell ref="AM33:AN33"/>
+    <mergeCell ref="AM34:AN34"/>
+    <mergeCell ref="AM35:AN35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>